<commit_message>
Final commit Thesis Chapter 7
</commit_message>
<xml_diff>
--- a/Traits/MesuredSpecimens67.xlsx
+++ b/Traits/MesuredSpecimens67.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/afe1_st-andrews_ac_uk/Documents/PHD/ThesisChapterMexico_I/TemporalChange_MexicanFish_C2/Traits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="8_{00423B5F-5BB1-4768-85F7-42D26E7FB13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7541976C-734E-4AE4-A192-BB1F55D46C1C}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="8_{00423B5F-5BB1-4768-85F7-42D26E7FB13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1041A1CB-672E-44ED-B1C8-B1EDE41CF1DF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="taxa - copy" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$O$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'taxa - copy'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3448" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3447" uniqueCount="768">
   <si>
     <t>Genus_species</t>
   </si>
@@ -2348,9 +2349,6 @@
     <t>rio Apamila , 4.5 km al oeste-noroeste de La Huerta, Son.</t>
   </si>
   <si>
-    <t>tornado de Regan (1906-1908: lam. 1, fig. 1),</t>
-  </si>
-  <si>
     <t>Green, copiado por P. Pelletier</t>
   </si>
   <si>
@@ -2385,9 +2383,6 @@
   </si>
   <si>
     <t>TU 30782</t>
-  </si>
-  <si>
-    <t>? Thursday 8th?</t>
   </si>
 </sst>
 </file>
@@ -2919,7 +2914,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -2969,10 +2964,6 @@
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" xfId="38"/>
     <xf numFmtId="14" fontId="17" fillId="29" borderId="0" xfId="38" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="38" borderId="0" xfId="38" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -14121,7 +14112,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection sqref="A1:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14137,536 +14128,536 @@
     <col min="14" max="14" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="47" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" t="s">
         <v>296</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" t="s">
         <v>297</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" t="s">
         <v>298</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" t="s">
         <v>302</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" t="s">
         <v>511</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" t="s">
         <v>611</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" t="s">
         <v>612</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" t="s">
         <v>615</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" t="s">
         <v>616</v>
       </c>
-      <c r="N1" s="47" t="s">
+      <c r="N1" t="s">
         <v>621</v>
       </c>
-      <c r="O1" s="47" t="s">
+      <c r="O1" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" t="s">
         <v>312</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" t="s">
         <v>305</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" t="s">
         <v>307</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H2" s="10">
+      <c r="F2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G2" t="s">
+        <v>303</v>
+      </c>
+      <c r="H2" s="1">
         <v>45363</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" t="s">
         <v>613</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" t="s">
         <v>677</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" t="s">
         <v>676</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" t="s">
         <v>326</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" t="s">
         <v>327</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" t="s">
         <v>310</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H3" s="10">
+      <c r="G3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H3" s="1">
         <v>45393</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" t="s">
         <v>717</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" t="s">
         <v>709</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" t="s">
         <v>613</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" t="s">
         <v>691</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" t="s">
         <v>687</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" t="s">
         <v>356</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" t="s">
         <v>326</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" t="s">
         <v>307</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H4" s="10">
+      <c r="F4" t="s">
+        <v>308</v>
+      </c>
+      <c r="G4" t="s">
+        <v>303</v>
+      </c>
+      <c r="H4" s="1">
         <v>45395</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" t="s">
         <v>713</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" t="s">
         <v>613</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" t="s">
         <v>714</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" t="s">
         <v>715</v>
       </c>
-      <c r="O4" s="9" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="O4" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" t="s">
         <v>395</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" t="s">
         <v>305</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" t="s">
         <v>327</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G5" s="9" t="s">
+      <c r="F5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G5" t="s">
         <v>310</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="1">
         <v>45512</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" t="s">
         <v>718</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" t="s">
         <v>613</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" t="s">
         <v>720</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" t="s">
         <v>721</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" t="s">
         <v>522</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" t="s">
         <v>326</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" t="s">
         <v>327</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H6" s="10">
+      <c r="F6" t="s">
+        <v>308</v>
+      </c>
+      <c r="G6" t="s">
+        <v>303</v>
+      </c>
+      <c r="H6" s="1">
         <v>45413</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" t="s">
         <v>613</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" t="s">
         <v>723</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" t="s">
         <v>687</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" t="s">
         <v>419</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" t="s">
         <v>326</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" t="s">
         <v>327</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H7" s="10">
+      <c r="F7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G7" t="s">
+        <v>303</v>
+      </c>
+      <c r="H7" s="1">
         <v>45399</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" t="s">
         <v>618</v>
       </c>
-      <c r="L7" s="50" t="s">
+      <c r="L7" t="s">
         <v>725</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" t="s">
         <v>643</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O7" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" t="s">
         <v>454</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" t="s">
         <v>305</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" t="s">
         <v>327</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" t="s">
         <v>310</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H8" s="10">
+      <c r="G8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H8" s="1">
         <v>45403</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" t="s">
         <v>613</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" t="s">
         <v>726</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N8" t="s">
         <v>643</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="O8" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>716</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" t="s">
         <v>265</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" t="s">
         <v>461</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" t="s">
         <v>305</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" t="s">
         <v>327</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" t="s">
         <v>310</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H9" s="10">
+      <c r="G9" t="s">
+        <v>303</v>
+      </c>
+      <c r="H9" s="1">
         <v>45404</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" t="s">
         <v>728</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" t="s">
         <v>613</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" t="s">
         <v>729</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="N9" t="s">
         <v>656</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" t="s">
         <v>456</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" t="s">
         <v>305</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" t="s">
         <v>327</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H10" s="10">
+      <c r="F10" t="s">
+        <v>308</v>
+      </c>
+      <c r="G10" t="s">
+        <v>303</v>
+      </c>
+      <c r="H10" s="1">
         <v>45403</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" t="s">
         <v>731</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" t="s">
         <v>618</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" t="s">
         <v>733</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N10" t="s">
         <v>656</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="O10" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" t="s">
         <v>457</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" t="s">
         <v>305</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" t="s">
         <v>327</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H11" s="10">
+      <c r="F11" t="s">
+        <v>308</v>
+      </c>
+      <c r="G11" t="s">
+        <v>303</v>
+      </c>
+      <c r="H11" s="1">
         <v>45403</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" t="s">
         <v>728</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" t="s">
         <v>613</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L11" t="s">
         <v>735</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="N11" t="s">
         <v>656</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" t="s">
         <v>458</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" t="s">
         <v>305</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" t="s">
         <v>327</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H12" s="10">
+      <c r="F12" t="s">
+        <v>308</v>
+      </c>
+      <c r="G12" t="s">
+        <v>303</v>
+      </c>
+      <c r="H12" s="1">
         <v>45403</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" t="s">
         <v>713</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" t="s">
         <v>613</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L12" t="s">
         <v>665</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="N12" t="s">
         <v>656</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="O12" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" t="s">
         <v>462</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" t="s">
         <v>305</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" t="s">
         <v>327</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" t="s">
         <v>310</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="H13" s="10">
+      <c r="G13" t="s">
+        <v>303</v>
+      </c>
+      <c r="H13" s="1">
         <v>45404</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" t="s">
         <v>736</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" t="s">
         <v>713</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" t="s">
         <v>613</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" t="s">
         <v>658</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="N13" t="s">
         <v>659</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" t="s">
         <v>660</v>
       </c>
     </row>
@@ -14695,16 +14686,16 @@
       <c r="H14" s="1">
         <v>45415</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" t="s">
         <v>613</v>
       </c>
-      <c r="L14" s="49" t="s">
+      <c r="L14" t="s">
         <v>737</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N14" t="s">
         <v>643</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="O14" t="s">
         <v>738</v>
       </c>
     </row>
@@ -14733,16 +14724,16 @@
       <c r="H15" s="1">
         <v>45415</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" t="s">
         <v>613</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L15" t="s">
         <v>739</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N15" t="s">
         <v>676</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="O15" t="s">
         <v>740</v>
       </c>
     </row>
@@ -14774,34 +14765,34 @@
       <c r="I16" t="s">
         <v>449</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" t="s">
         <v>613</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="L16" t="s">
         <v>742</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N16" t="s">
         <v>643</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="O16" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>712</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>196</v>
       </c>
       <c r="C17" t="s">
-        <v>543</v>
+        <v>601</v>
       </c>
       <c r="D17" t="s">
         <v>326</v>
       </c>
       <c r="E17" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="F17" t="s">
         <v>308</v>
@@ -14810,39 +14801,39 @@
         <v>303</v>
       </c>
       <c r="H17" s="1">
-        <v>45408</v>
+        <v>45424</v>
       </c>
       <c r="I17" t="s">
-        <v>540</v>
-      </c>
-      <c r="K17" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="K17" t="s">
         <v>613</v>
       </c>
-      <c r="L17" s="49" t="s">
-        <v>744</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>672</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>743</v>
+      <c r="L17" t="s">
+        <v>745</v>
+      </c>
+      <c r="N17" t="s">
+        <v>694</v>
+      </c>
+      <c r="O17" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>712</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s">
-        <v>601</v>
+        <v>460</v>
       </c>
       <c r="D18" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="E18" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="F18" t="s">
         <v>308</v>
@@ -14851,39 +14842,36 @@
         <v>303</v>
       </c>
       <c r="H18" s="1">
-        <v>45424</v>
-      </c>
-      <c r="I18" t="s">
-        <v>602</v>
-      </c>
-      <c r="K18" s="9" t="s">
+        <v>45403</v>
+      </c>
+      <c r="K18" t="s">
         <v>613</v>
       </c>
-      <c r="L18" s="9" t="s">
-        <v>745</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>694</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>746</v>
+      <c r="L18" t="s">
+        <v>748</v>
+      </c>
+      <c r="N18" t="s">
+        <v>676</v>
+      </c>
+      <c r="O18" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>711</v>
       </c>
       <c r="B19" t="s">
-        <v>174</v>
+        <v>270</v>
       </c>
       <c r="C19" t="s">
-        <v>460</v>
+        <v>348</v>
       </c>
       <c r="D19" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="E19" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="F19" t="s">
         <v>308</v>
@@ -14892,19 +14880,22 @@
         <v>303</v>
       </c>
       <c r="H19" s="1">
-        <v>45403</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="L19" s="9" t="s">
-        <v>748</v>
-      </c>
-      <c r="N19" s="9" t="s">
-        <v>676</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>747</v>
+        <v>45363</v>
+      </c>
+      <c r="I19" t="s">
+        <v>349</v>
+      </c>
+      <c r="K19" t="s">
+        <v>618</v>
+      </c>
+      <c r="L19" t="s">
+        <v>762</v>
+      </c>
+      <c r="N19" t="s">
+        <v>687</v>
+      </c>
+      <c r="O19" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
@@ -14932,16 +14923,16 @@
       <c r="H20" s="1">
         <v>45406</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="K20" t="s">
         <v>613</v>
       </c>
-      <c r="L20" s="9" t="s">
+      <c r="L20" t="s">
         <v>749</v>
       </c>
-      <c r="N20" s="9" t="s">
+      <c r="N20" t="s">
         <v>648</v>
       </c>
-      <c r="O20" s="9" t="s">
+      <c r="O20" t="s">
         <v>750</v>
       </c>
     </row>
@@ -14973,16 +14964,16 @@
       <c r="I21" t="s">
         <v>565</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" t="s">
         <v>618</v>
       </c>
-      <c r="L21" s="9" t="s">
+      <c r="L21" t="s">
         <v>751</v>
       </c>
-      <c r="N21" s="9" t="s">
+      <c r="N21" t="s">
         <v>694</v>
       </c>
-      <c r="O21" s="9" t="s">
+      <c r="O21" t="s">
         <v>753</v>
       </c>
     </row>
@@ -15011,31 +15002,31 @@
       <c r="H22" s="1">
         <v>45424</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K22" t="s">
         <v>613</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="L22" t="s">
         <v>755</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="N22" t="s">
         <v>754</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="O22" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B23" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C23" t="s">
-        <v>342</v>
+        <v>543</v>
       </c>
       <c r="D23" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
       <c r="E23" t="s">
         <v>307</v>
@@ -15047,36 +15038,39 @@
         <v>303</v>
       </c>
       <c r="H23" s="1">
-        <v>45364</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="L23" s="9" t="s">
-        <v>758</v>
-      </c>
-      <c r="N23" s="9" t="s">
-        <v>757</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>756</v>
+        <v>45408</v>
+      </c>
+      <c r="I23" t="s">
+        <v>540</v>
+      </c>
+      <c r="K23" t="s">
+        <v>613</v>
+      </c>
+      <c r="L23" t="s">
+        <v>744</v>
+      </c>
+      <c r="N23" t="s">
+        <v>672</v>
+      </c>
+      <c r="O23" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B24" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C24" t="s">
-        <v>496</v>
+        <v>342</v>
       </c>
       <c r="D24" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="E24" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="F24" t="s">
         <v>308</v>
@@ -15085,33 +15079,33 @@
         <v>303</v>
       </c>
       <c r="H24" s="1">
-        <v>45406</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="L24" s="9" t="s">
-        <v>761</v>
-      </c>
-      <c r="N24" s="9" t="s">
-        <v>687</v>
-      </c>
-      <c r="O24" s="9" t="s">
-        <v>760</v>
+        <v>45364</v>
+      </c>
+      <c r="K24" t="s">
+        <v>618</v>
+      </c>
+      <c r="L24" t="s">
+        <v>757</v>
+      </c>
+      <c r="N24" t="s">
+        <v>756</v>
+      </c>
+      <c r="O24" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>711</v>
+        <v>256</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C25" t="s">
-        <v>348</v>
+        <v>496</v>
       </c>
       <c r="D25" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="E25" t="s">
         <v>327</v>
@@ -15123,22 +15117,19 @@
         <v>303</v>
       </c>
       <c r="H25" s="1">
-        <v>45363</v>
-      </c>
-      <c r="I25" t="s">
-        <v>349</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="L25" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="N25" s="9" t="s">
+        <v>45406</v>
+      </c>
+      <c r="K25" t="s">
+        <v>613</v>
+      </c>
+      <c r="L25" t="s">
+        <v>760</v>
+      </c>
+      <c r="N25" t="s">
         <v>687</v>
       </c>
-      <c r="O25" s="9" t="s">
-        <v>762</v>
+      <c r="O25" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
@@ -15163,20 +15154,20 @@
       <c r="G26" t="s">
         <v>303</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>769</v>
-      </c>
-      <c r="K26" s="9" t="s">
+      <c r="H26" s="1">
+        <v>45512</v>
+      </c>
+      <c r="K26" t="s">
         <v>613</v>
       </c>
-      <c r="L26" s="49" t="s">
-        <v>765</v>
-      </c>
-      <c r="N26" s="9" t="s">
+      <c r="L26" t="s">
+        <v>764</v>
+      </c>
+      <c r="N26" t="s">
         <v>687</v>
       </c>
-      <c r="O26" s="9" t="s">
-        <v>764</v>
+      <c r="O26" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
@@ -15204,17 +15195,17 @@
       <c r="H27" s="1">
         <v>45437</v>
       </c>
-      <c r="K27" s="9" t="s">
+      <c r="K27" t="s">
         <v>613</v>
       </c>
-      <c r="L27" s="9" t="s">
-        <v>767</v>
-      </c>
-      <c r="N27" s="9" t="s">
+      <c r="L27" t="s">
+        <v>766</v>
+      </c>
+      <c r="N27" t="s">
         <v>687</v>
       </c>
-      <c r="O27" s="9" t="s">
-        <v>766</v>
+      <c r="O27" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
@@ -15242,17 +15233,17 @@
       <c r="H28" s="1">
         <v>45397</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K28" t="s">
         <v>613</v>
       </c>
-      <c r="L28" s="9" t="s">
+      <c r="L28" t="s">
         <v>729</v>
       </c>
-      <c r="N28" s="9" t="s">
+      <c r="N28" t="s">
         <v>676</v>
       </c>
-      <c r="O28" s="9" t="s">
-        <v>768</v>
+      <c r="O28" t="s">
+        <v>767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>